<commit_message>
-solve problem in dashboard & change chart diagram
</commit_message>
<xml_diff>
--- a/public/excel/user (1).xlsx
+++ b/public/excel/user (1).xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView windowWidth="23040" windowHeight="9924"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
   <si>
     <t>Nama</t>
   </si>
@@ -71,79 +70,430 @@
     <t>Pekerjaan Ibu</t>
   </si>
   <si>
-    <t>Daffa</t>
-  </si>
-  <si>
-    <t>daffa@gmail.com</t>
-  </si>
-  <si>
-    <t>0058583536</t>
+    <t>Armand Nur</t>
+  </si>
+  <si>
+    <t>Teknik Komputer dan Jaringan</t>
+  </si>
+  <si>
+    <t>zxuanggg@gmail.com</t>
   </si>
   <si>
     <t>Gg. Syawal Street Rt0607 no.26</t>
   </si>
   <si>
+    <t>kerja</t>
+  </si>
+  <si>
+    <t>085163562456</t>
+  </si>
+  <si>
+    <t>Jakarta</t>
+  </si>
+  <si>
+    <t>laki-laki</t>
+  </si>
+  <si>
+    <t>menikah</t>
+  </si>
+  <si>
+    <t>EKO</t>
+  </si>
+  <si>
+    <t>Tri</t>
+  </si>
+  <si>
+    <t>Kantoran</t>
+  </si>
+  <si>
+    <t>IRT</t>
+  </si>
+  <si>
+    <t>Dias</t>
+  </si>
+  <si>
+    <t>Sucipto</t>
+  </si>
+  <si>
+    <t>Ika</t>
+  </si>
+  <si>
+    <t>Nanda</t>
+  </si>
+  <si>
     <t>kuliah</t>
   </si>
   <si>
-    <t>085163562456</t>
-  </si>
-  <si>
-    <t>Jakarta</t>
-  </si>
-  <si>
-    <t>2023-05-01</t>
-  </si>
-  <si>
-    <t>laki-laki</t>
-  </si>
-  <si>
-    <t>menikah</t>
-  </si>
-  <si>
-    <t>PT. Intertek</t>
-  </si>
-  <si>
-    <t>UGM</t>
-  </si>
-  <si>
-    <t>EKO</t>
-  </si>
-  <si>
-    <t>Tri</t>
-  </si>
-  <si>
-    <t>Kantoran</t>
-  </si>
-  <si>
-    <t>IRT</t>
+    <t>Topiq</t>
+  </si>
+  <si>
+    <t>Sri</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -151,18 +501,313 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -447,41 +1092,36 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:R2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="1" width="6.998" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="9.283" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="18.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="36.42" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="10.569" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="8.141" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="15.282" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="15.282" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="16.425" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="16.425" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="21.138" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="15.282" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="16.425" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="11.711" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="10.569" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="12.8518518518519" customWidth="1"/>
+    <col min="2" max="2" width="34.1388888888889" customWidth="1"/>
+    <col min="3" max="3" width="22.2777777777778" customWidth="1"/>
+    <col min="4" max="4" width="8.13888888888889" customWidth="1"/>
+    <col min="5" max="5" width="36.4166666666667" customWidth="1"/>
+    <col min="6" max="6" width="10.5648148148148" customWidth="1"/>
+    <col min="7" max="7" width="8.13888888888889" customWidth="1"/>
+    <col min="8" max="9" width="15.2777777777778" customWidth="1"/>
+    <col min="10" max="11" width="16.4259259259259" customWidth="1"/>
+    <col min="12" max="12" width="21.1388888888889" customWidth="1"/>
+    <col min="13" max="13" width="15.2777777777778" customWidth="1"/>
+    <col min="14" max="14" width="16.4259259259259" customWidth="1"/>
+    <col min="15" max="15" width="11.712962962963" customWidth="1"/>
+    <col min="16" max="16" width="10.5648148148148" customWidth="1"/>
+    <col min="17" max="17" width="17.5648148148148" customWidth="1"/>
+    <col min="18" max="18" width="16.4259259259259" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -544,11 +1184,14 @@
       <c r="A2" t="s">
         <v>18</v>
       </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
       <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
         <v>20</v>
+      </c>
+      <c r="D2">
+        <v>123321</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>
@@ -565,46 +1208,125 @@
       <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1">
+        <v>45282</v>
+      </c>
+      <c r="K2" t="s">
         <v>25</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>26</v>
       </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
         <v>27</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>28</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" t="s">
         <v>29</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R2" t="s">
         <v>30</v>
       </c>
-      <c r="P2" t="s">
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>234432</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3">
+        <v>2001</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="1">
+        <v>45282</v>
+      </c>
+      <c r="K3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" t="s">
         <v>32</v>
       </c>
-      <c r="R2" t="s">
+      <c r="P3" t="s">
         <v>33</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>29</v>
+      </c>
+      <c r="R3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>345543</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4">
+        <v>2002</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1">
+        <v>45282</v>
+      </c>
+      <c r="K4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>